<commit_message>
actualizando ieee830 segun avances y cambios de sprint 1
</commit_message>
<xml_diff>
--- a/docs/planilla-us/Historias Usuario ClinicFlow.xlsx
+++ b/docs/planilla-us/Historias Usuario ClinicFlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="449">
   <si>
     <t>Historias de usuario y criterios de aceptación: Ejemplo</t>
   </si>
@@ -1311,12 +1311,21 @@
     <t>Diseñar y subir script SQL de la base de datos (MySQL).</t>
   </si>
   <si>
+    <t>Mike</t>
+  </si>
+  <si>
     <t>Crear módulo Python para conexión a MySQL.</t>
   </si>
   <si>
+    <t>Mike, Tomas</t>
+  </si>
+  <si>
     <t>Implementar función de registro de usuario por consola.</t>
   </si>
   <si>
+    <t>Mike, Vir</t>
+  </si>
+  <si>
     <t>Como cliente, quiero iniciar sesión mediante consola con mis credenciales registradas para poder realizar las tareas que necesito.</t>
   </si>
   <si>
@@ -1341,10 +1350,16 @@
     <t>Implementar función para visualizar y editar datos de usuario (consola).</t>
   </si>
   <si>
+    <t>Vir</t>
+  </si>
+  <si>
     <t>Como administrador, quiero poder listar todos los usuarios registrados, cambiar roles y eliminar cuentas, para poder gestionarlos.</t>
   </si>
   <si>
     <t>Implementar función para listar usuarios (solo admin).</t>
+  </si>
+  <si>
+    <t>Tomas</t>
   </si>
   <si>
     <t>Implementar función para cambiar rol de usuario (solo admin).</t>
@@ -1685,7 +1700,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1950,9 +1965,6 @@
     <xf borderId="27" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
@@ -1972,7 +1984,7 @@
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -26453,30 +26465,30 @@
     </row>
   </sheetData>
   <mergeCells count="122">
+    <mergeCell ref="K46:K49"/>
+    <mergeCell ref="L46:L49"/>
+    <mergeCell ref="K51:K54"/>
+    <mergeCell ref="L51:L54"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="L56:L59"/>
     <mergeCell ref="L61:L64"/>
+    <mergeCell ref="K61:K64"/>
+    <mergeCell ref="K66:K69"/>
     <mergeCell ref="L66:L69"/>
+    <mergeCell ref="K71:K74"/>
     <mergeCell ref="L71:L74"/>
+    <mergeCell ref="K76:K79"/>
     <mergeCell ref="L76:L79"/>
-    <mergeCell ref="L96:L99"/>
-    <mergeCell ref="L101:L104"/>
-    <mergeCell ref="L81:L84"/>
-    <mergeCell ref="L86:L89"/>
-    <mergeCell ref="L91:L94"/>
-    <mergeCell ref="L51:L54"/>
-    <mergeCell ref="K51:K54"/>
-    <mergeCell ref="L46:L49"/>
-    <mergeCell ref="L56:L59"/>
-    <mergeCell ref="K46:K49"/>
-    <mergeCell ref="K61:K64"/>
-    <mergeCell ref="K91:K94"/>
     <mergeCell ref="K96:K99"/>
     <mergeCell ref="K101:K104"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="K66:K69"/>
-    <mergeCell ref="K71:K74"/>
-    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="L101:L104"/>
     <mergeCell ref="K81:K84"/>
+    <mergeCell ref="L81:L84"/>
     <mergeCell ref="K86:K89"/>
+    <mergeCell ref="L86:L89"/>
+    <mergeCell ref="K91:K94"/>
+    <mergeCell ref="L91:L94"/>
+    <mergeCell ref="L96:L99"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="C6:C9"/>
@@ -26493,26 +26505,26 @@
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
+    <mergeCell ref="K11:K14"/>
+    <mergeCell ref="L11:L14"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="L26:L29"/>
     <mergeCell ref="D36:D39"/>
     <mergeCell ref="E36:E39"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="C41:C44"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="E41:E44"/>
-    <mergeCell ref="L26:L29"/>
+    <mergeCell ref="K26:K29"/>
+    <mergeCell ref="K31:K34"/>
     <mergeCell ref="L31:L34"/>
+    <mergeCell ref="K36:K39"/>
     <mergeCell ref="L36:L39"/>
+    <mergeCell ref="K41:K44"/>
     <mergeCell ref="L41:L44"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="K31:K34"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="K41:K44"/>
-    <mergeCell ref="K26:K29"/>
-    <mergeCell ref="K11:K14"/>
-    <mergeCell ref="L11:L14"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L21:L24"/>
     <mergeCell ref="B66:B69"/>
     <mergeCell ref="C66:C69"/>
     <mergeCell ref="D66:D69"/>
@@ -31110,7 +31122,9 @@
       <c r="D12" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="E12" s="96"/>
+      <c r="E12" s="92" t="s">
+        <v>430</v>
+      </c>
       <c r="F12" s="93"/>
       <c r="G12" s="79" t="s">
         <v>37</v>
@@ -31123,9 +31137,11 @@
         <v>390</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>430</v>
-      </c>
-      <c r="E13" s="96"/>
+        <v>431</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>432</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
@@ -31136,9 +31152,11 @@
         <v>378</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>431</v>
-      </c>
-      <c r="E14" s="96"/>
+        <v>433</v>
+      </c>
+      <c r="E14" s="92" t="s">
+        <v>434</v>
+      </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
@@ -31147,15 +31165,17 @@
         <v>224</v>
       </c>
       <c r="B15" s="91" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C15" s="75" t="s">
         <v>402</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>433</v>
-      </c>
-      <c r="E15" s="96"/>
+        <v>436</v>
+      </c>
+      <c r="E15" s="92" t="s">
+        <v>434</v>
+      </c>
       <c r="F15" s="93"/>
       <c r="G15" s="79" t="s">
         <v>37</v>
@@ -31168,92 +31188,104 @@
         <v>404</v>
       </c>
       <c r="D16" s="27" t="s">
+        <v>437</v>
+      </c>
+      <c r="E16" s="92" t="s">
         <v>434</v>
       </c>
-      <c r="E16" s="96"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="96" t="s">
         <v>279</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>437</v>
-      </c>
-      <c r="E17" s="96"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="99" t="s">
+        <v>440</v>
+      </c>
+      <c r="E17" s="92" t="s">
+        <v>432</v>
+      </c>
+      <c r="F17" s="97"/>
+      <c r="G17" s="98" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" ht="72.75" customHeight="1">
-      <c r="A18" s="97" t="s">
+      <c r="A18" s="96" t="s">
         <v>327</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C18" s="84" t="s">
         <v>406</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>439</v>
-      </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="99" t="s">
+        <v>442</v>
+      </c>
+      <c r="E18" s="92" t="s">
+        <v>443</v>
+      </c>
+      <c r="F18" s="97"/>
+      <c r="G18" s="98" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="99" t="s">
         <v>341</v>
       </c>
-      <c r="B19" s="101" t="s">
-        <v>440</v>
-      </c>
-      <c r="C19" s="102" t="s">
+      <c r="B19" s="100" t="s">
+        <v>444</v>
+      </c>
+      <c r="C19" s="101" t="s">
         <v>409</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>441</v>
-      </c>
-      <c r="E19" s="103"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="105" t="s">
+        <v>445</v>
+      </c>
+      <c r="E19" s="102" t="s">
+        <v>446</v>
+      </c>
+      <c r="F19" s="103"/>
+      <c r="G19" s="104" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="80"/>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="105" t="s">
         <v>412</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="E20" s="103"/>
+        <v>447</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>446</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
     <row r="21" ht="46.5" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="82"/>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="105" t="s">
         <v>375</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>443</v>
-      </c>
-      <c r="E21" s="103"/>
+        <v>448</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>446</v>
+      </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
@@ -35151,6 +35183,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="F4:F7"/>
@@ -35158,23 +35198,15 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>